<commit_message>
test plan: added some executed tests about factory default setting
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan_20200915.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan_20200915.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="814" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" tabRatio="814" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_His." sheetId="3" r:id="rId1"/>
@@ -805,7 +805,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="299">
   <si>
     <t>Test ID</t>
   </si>
@@ -1074,9 +1074,6 @@
   </si>
   <si>
     <t>1. GME regularly running</t>
-  </si>
-  <si>
-    <t>NECESSARIO CAPIRE SE PUO' ESSERE FATTO PARTIRE IN OGNI MOMENTO O SOLO AL BOOT, DA VALUTARE INSIEME AL SECURE BOOT</t>
   </si>
   <si>
     <t>1. the device is powered off
@@ -2067,6 +2064,12 @@
   </si>
   <si>
     <t>1. the red led is ON</t>
+  </si>
+  <si>
+    <t>factory default config can be set at any time</t>
+  </si>
+  <si>
+    <t>after factory, GME restarts with default configuration</t>
   </si>
 </sst>
 </file>
@@ -3275,10 +3278,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
@@ -3287,10 +3290,10 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -3401,10 +3404,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3412,25 +3415,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>180</v>
-      </c>
       <c r="D2" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="48">
         <v>44047</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3439,25 +3442,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G3" s="48">
         <v>44069</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3466,25 +3469,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G4" s="48">
         <v>44089</v>
       </c>
       <c r="H4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3493,19 +3496,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3514,13 +3517,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="16" t="s">
         <v>182</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>183</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7</v>
@@ -3529,7 +3532,7 @@
         <v>44047</v>
       </c>
       <c r="H6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -3538,12 +3541,12 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="16"/>
       <c r="E7" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -3552,73 +3555,73 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G8" s="48">
         <v>44089</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>194</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>195</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G9" s="48">
         <v>44069</v>
       </c>
       <c r="H9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G10" s="48">
         <v>44069</v>
       </c>
       <c r="H10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="259.2" x14ac:dyDescent="0.3">
@@ -3627,7 +3630,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
@@ -3635,13 +3638,13 @@
         <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G11" s="48">
         <v>44047</v>
       </c>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -3650,7 +3653,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="16"/>
@@ -4002,8 +4005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4038,13 +4041,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -4055,9 +4058,17 @@
         <v>77</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="48"/>
+        <v>297</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="48">
+        <v>44089</v>
+      </c>
+      <c r="H2" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
@@ -4070,7 +4081,18 @@
       <c r="C3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="48">
+        <v>44089</v>
+      </c>
+      <c r="H3" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
@@ -4474,10 +4496,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -4494,7 +4516,7 @@
         <v>38</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G2" s="48"/>
     </row>
@@ -4726,7 +4748,7 @@
         <v>44077</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4750,7 +4772,7 @@
         <v>44077</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4759,7 +4781,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>67</v>
@@ -4771,13 +4793,13 @@
         <v>7</v>
       </c>
       <c r="F18" s="47" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G18" s="49">
         <v>44077</v>
       </c>
       <c r="H18" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -4795,10 +4817,10 @@
         <v>71</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -4822,7 +4844,7 @@
         <v>44077</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4843,13 +4865,13 @@
         <v>7</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G21" s="49">
         <v>44077</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5078,10 +5100,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -5089,13 +5111,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>215</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>216</v>
       </c>
       <c r="G2" s="48"/>
     </row>
@@ -5505,7 +5527,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -5627,10 +5649,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5638,13 +5660,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>202</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7</v>
@@ -5653,7 +5675,7 @@
         <v>44047</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5662,13 +5684,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>205</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7</v>
@@ -5677,7 +5699,7 @@
         <v>44047</v>
       </c>
       <c r="H3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -5695,13 +5717,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>202</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7</v>
@@ -5710,7 +5732,7 @@
         <v>44047</v>
       </c>
       <c r="H5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5719,13 +5741,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>205</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7</v>
@@ -5734,7 +5756,7 @@
         <v>44047</v>
       </c>
       <c r="H6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -6146,10 +6168,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6157,25 +6179,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="16" t="s">
         <v>209</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>210</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G2" s="48">
         <v>44077</v>
       </c>
       <c r="H2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6184,13 +6206,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>212</v>
-      </c>
       <c r="D3" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7</v>
@@ -6200,7 +6222,7 @@
         <v>44077</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -6209,13 +6231,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>255</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>256</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7</v>
@@ -6224,7 +6246,7 @@
         <v>44077</v>
       </c>
       <c r="H4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6233,13 +6255,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>258</v>
-      </c>
       <c r="D5" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7</v>
@@ -6248,7 +6270,7 @@
         <v>44077</v>
       </c>
       <c r="H5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -6257,19 +6279,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>222</v>
-      </c>
       <c r="E6" s="11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -6671,10 +6693,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6682,13 +6704,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>223</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>224</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7</v>
@@ -6697,7 +6719,7 @@
         <v>44047</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -6706,16 +6728,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>227</v>
-      </c>
       <c r="D3" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -6724,25 +6746,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>229</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>230</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G4" s="48">
         <v>44047</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -6751,25 +6773,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>231</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>232</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G5" s="48">
         <v>44047</v>
       </c>
       <c r="H5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -7157,10 +7179,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -7171,7 +7193,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>27</v>
@@ -7183,7 +7205,7 @@
         <v>44047</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -7198,7 +7220,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7</v>
@@ -7207,7 +7229,7 @@
         <v>44047</v>
       </c>
       <c r="H3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -7222,19 +7244,19 @@
         <v>13</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G4" s="48">
         <v>44047</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -7583,7 +7605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -7619,10 +7641,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -7633,22 +7655,22 @@
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G2" s="48">
         <v>44047</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -7660,10 +7682,10 @@
         <v>16</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>7</v>
@@ -7673,7 +7695,7 @@
         <v>44047</v>
       </c>
       <c r="H3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -7688,19 +7710,19 @@
         <v>14</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G4" s="48">
         <v>44047</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -7709,13 +7731,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>101</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>102</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7</v>
@@ -7724,7 +7746,7 @@
         <v>44047</v>
       </c>
       <c r="H5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -7733,13 +7755,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7</v>
@@ -7748,7 +7770,7 @@
         <v>44047</v>
       </c>
       <c r="H6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -7760,10 +7782,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>7</v>
@@ -7772,7 +7794,7 @@
         <v>44047</v>
       </c>
       <c r="H7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -7781,13 +7803,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>7</v>
@@ -7796,7 +7818,7 @@
         <v>44047</v>
       </c>
       <c r="H8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -7805,25 +7827,25 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>218</v>
-      </c>
       <c r="D9" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G9" s="48">
         <v>44077</v>
       </c>
       <c r="H9" s="50" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -7832,13 +7854,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>7</v>
@@ -7847,7 +7869,7 @@
         <v>44047</v>
       </c>
       <c r="H10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -7856,25 +7878,25 @@
         <v>10</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G11" s="49">
         <v>44075</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -7883,25 +7905,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>198</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>199</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G12" s="51">
         <v>44075</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -7910,25 +7932,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>95</v>
-      </c>
       <c r="D13" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G13" s="49">
         <v>44076</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -7940,10 +7962,10 @@
         <v>29</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>7</v>
@@ -7952,7 +7974,7 @@
         <v>44047</v>
       </c>
       <c r="H14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -7961,13 +7983,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>107</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>108</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>7</v>
@@ -7976,7 +7998,7 @@
         <v>44047</v>
       </c>
       <c r="H15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -7985,13 +8007,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>109</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>7</v>
@@ -8000,7 +8022,7 @@
         <v>44047</v>
       </c>
       <c r="H16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -8009,25 +8031,25 @@
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>114</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>115</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G17" s="49">
         <v>44077</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
@@ -8036,23 +8058,23 @@
         <v>17</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G18" s="49">
         <v>44070</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -8400,10 +8422,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="35" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -8411,25 +8433,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>234</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>236</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>235</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G2" s="48">
         <v>44047</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:8" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8437,17 +8459,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>237</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>238</v>
       </c>
       <c r="E3" s="34"/>
       <c r="F3" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
@@ -8457,25 +8479,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="38" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>243</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>244</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G4" s="48">
         <v>44047</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -8483,25 +8505,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="C5" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="D5" s="37" t="s">
         <v>269</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>270</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G5" s="48">
         <v>44077</v>
       </c>
       <c r="H5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.3">
@@ -9901,10 +9923,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="144" x14ac:dyDescent="0.3">
@@ -9913,7 +9935,7 @@
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" s="16"/>
       <c r="G2" s="48"/>
@@ -9924,13 +9946,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>7</v>
@@ -9939,7 +9961,7 @@
         <v>44047</v>
       </c>
       <c r="H3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -9948,13 +9970,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>117</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>118</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>7</v>
@@ -9963,7 +9985,7 @@
         <v>44047</v>
       </c>
       <c r="H4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -9972,13 +9994,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>120</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>121</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>7</v>
@@ -9987,7 +10009,7 @@
         <v>44047</v>
       </c>
       <c r="H5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -9996,13 +10018,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="D6" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>7</v>
@@ -10011,7 +10033,7 @@
         <v>44047</v>
       </c>
       <c r="H6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
@@ -10020,13 +10042,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>125</v>
-      </c>
       <c r="D7" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>7</v>
@@ -10036,7 +10058,7 @@
         <v>44047</v>
       </c>
       <c r="H7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -10045,13 +10067,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>136</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>137</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>7</v>
@@ -10060,7 +10082,7 @@
         <v>44047</v>
       </c>
       <c r="H8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="158.4" x14ac:dyDescent="0.3">
@@ -10069,13 +10091,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>7</v>
@@ -10084,7 +10106,7 @@
         <v>44047</v>
       </c>
       <c r="H9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
@@ -10093,25 +10115,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>140</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>141</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G10" s="48">
         <v>44047</v>
       </c>
       <c r="H10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -10120,25 +10142,25 @@
         <v>9</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>151</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G11" s="48">
         <v>44047</v>
       </c>
       <c r="H11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -10147,25 +10169,25 @@
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>152</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>153</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G12" s="51">
         <v>44077</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -10174,25 +10196,25 @@
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G13" s="49">
         <v>44077</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -10201,13 +10223,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>7</v>
@@ -10217,7 +10239,7 @@
         <v>44047</v>
       </c>
       <c r="H14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -10226,13 +10248,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>7</v>
@@ -10241,7 +10263,7 @@
         <v>44047</v>
       </c>
       <c r="H15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -10250,25 +10272,25 @@
         <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C16" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>145</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G16" s="48">
         <v>44047</v>
       </c>
       <c r="H16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -10277,25 +10299,25 @@
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>146</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>147</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G17" s="48">
         <v>44047</v>
       </c>
       <c r="H17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="6" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -10304,13 +10326,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>162</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>7</v>
@@ -10319,7 +10341,7 @@
         <v>44047</v>
       </c>
       <c r="H18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="6" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -10328,13 +10350,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>7</v>
@@ -10343,7 +10365,7 @@
         <v>44047</v>
       </c>
       <c r="H19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="6" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -10352,13 +10374,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>164</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>7</v>
@@ -10367,7 +10389,7 @@
         <v>44047</v>
       </c>
       <c r="H20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -10376,13 +10398,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21" s="12"/>
       <c r="G21" s="8"/>
@@ -10397,7 +10419,7 @@
         <v>30</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="12"/>
@@ -10408,10 +10430,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
@@ -10424,7 +10446,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="18"/>

</xml_diff>